<commit_message>
author : subhadra Comment :TasksBreakDown excel sheet updated.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/subhadra.xlsx
+++ b/TeamDetails/TasksBreakDown/subhadra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Story ID</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Understanding the concept of CSS</t>
   </si>
   <si>
-    <t>Make block diagram of the entire code journey(work flow)</t>
-  </si>
-  <si>
-    <t>Technical understanding(bootstrap)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Create structure of login page using html and css </t>
   </si>
   <si>
@@ -94,6 +88,15 @@
   </si>
   <si>
     <t>Task-7</t>
+  </si>
+  <si>
+    <t>Understanding Angular JS</t>
+  </si>
+  <si>
+    <t>Integrate structure of login page with angular js functionality</t>
+  </si>
+  <si>
+    <t>Total time</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -178,24 +181,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -213,16 +203,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2808,7 +2792,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,147 +2832,159 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <f>SUM(E2:E8)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2">
         <f>E2-F2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G45" si="0">E3-F3</f>
+        <f>(E3-F3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4" s="6">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f>(E4-F4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="6">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>(E5-F5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="9"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6">
         <v>4</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="6">
+        <v>3</v>
+      </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>E6-F6</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="E7" s="6">
+        <v>4</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>E7-F7</f>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="7">
-        <v>6</v>
+      <c r="E8" s="6">
+        <v>3</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>E8-F8</f>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6">
+        <f>SUM(E2:E8)</f>
+        <v>19</v>
+      </c>
+      <c r="F9" s="6">
+        <f>SUM(F2:F8)</f>
+        <v>10</v>
+      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -2998,7 +2994,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G6:G45" si="0">E10-F10</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author :Subhadra comment :subhadra.xlsx sheet updated.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/subhadra.xlsx
+++ b/TeamDetails/TasksBreakDown/subhadra.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Story ID</t>
   </si>
@@ -87,16 +87,28 @@
     <t>Task-6</t>
   </si>
   <si>
-    <t>Task-7</t>
-  </si>
-  <si>
     <t>Understanding Angular JS</t>
   </si>
   <si>
-    <t>Integrate structure of login page with angular js functionality</t>
+    <t>Total time</t>
   </si>
   <si>
-    <t>Total time</t>
+    <t>Develop complete understanding on the basis of requirement and acceptance criteria</t>
+  </si>
+  <si>
+    <t>Prepare test-cases for story SSDMS-2,4,5</t>
+  </si>
+  <si>
+    <t>Prepare test-cases for story SSDMS-6,7,8</t>
+  </si>
+  <si>
+    <t>Prepare test-cases for story SSDMS-9,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Test story SSDMS-1,3,4</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,11 +193,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -203,10 +228,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2791,8 +2828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,9 +2869,9 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="8">
         <f>SUM(E2:E8)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
@@ -2855,7 +2892,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
@@ -2875,7 +2912,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
@@ -2895,7 +2932,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
@@ -2915,7 +2952,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="8"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2935,38 +2972,34 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="6">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
       <c r="G7" s="2">
         <f>E7-F7</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="6">
-        <v>3</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
         <f>E8-F8</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2974,15 +3007,15 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6">
         <f>SUM(E2:E8)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F9" s="6">
         <f>SUM(F2:F8)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -2994,7 +3027,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f t="shared" ref="G6:G45" si="0">E10-F10</f>
+        <f t="shared" ref="G10:G45" si="0">E10-F10</f>
         <v>0</v>
       </c>
     </row>
@@ -3010,25 +3043,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="B12" s="8">
+        <f>SUM(E12:E16)</f>
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="11">
+        <v>4</v>
+      </c>
+      <c r="F12" s="11">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="11">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4</v>
+      </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3036,11 +3088,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4</v>
+      </c>
+      <c r="F14" s="6">
+        <v>4</v>
+      </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3048,11 +3108,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>3</v>
+      </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3060,26 +3128,40 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="6">
+        <f>SUM(E11:E16)</f>
+        <v>21</v>
+      </c>
+      <c r="F17" s="6">
+        <f>SUM(F12:F15)</f>
+        <v>15</v>
+      </c>
       <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3419,8 +3501,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:B8"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B12:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>